<commit_message>
Added symbolTally obj literal, result tiles and power button
</commit_message>
<xml_diff>
--- a/The Devil's Faire/Assets/images/SlotMachineAssetDetails.xlsx
+++ b/The Devil's Faire/Assets/images/SlotMachineAssetDetails.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jay\Documents\Visual Studio 2013\Projects\The-Devil-s-Faire\The Devil's Faire\Assets\images\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20484" windowHeight="15360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="158000" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
   <si>
     <t>X</t>
   </si>
@@ -108,18 +113,6 @@
     <t>PaleYellow</t>
   </si>
   <si>
-    <t>RJust.130x29</t>
-  </si>
-  <si>
-    <t>LJust.42x29</t>
-  </si>
-  <si>
-    <t>LJust.688x29</t>
-  </si>
-  <si>
-    <t>RJust.721x29</t>
-  </si>
-  <si>
     <t>WalletText</t>
   </si>
   <si>
@@ -132,12 +125,6 @@
     <t>DarkMustard</t>
   </si>
   <si>
-    <t>RJust.345x92</t>
-  </si>
-  <si>
-    <t>RJust.441x92</t>
-  </si>
-  <si>
     <t>JackpotWinnerText</t>
   </si>
   <si>
@@ -157,6 +144,18 @@
   </si>
   <si>
     <t>Background_fade</t>
+  </si>
+  <si>
+    <t>LJust.688x27</t>
+  </si>
+  <si>
+    <t>20px Arial</t>
+  </si>
+  <si>
+    <t>LJust.42x27</t>
+  </si>
+  <si>
+    <t>RJust.345x90</t>
   </si>
 </sst>
 </file>
@@ -310,6 +309,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -570,7 +572,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -578,13 +580,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:E29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -629,7 +631,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>800</v>
@@ -980,7 +982,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B24">
         <v>320</v>
@@ -997,7 +999,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B25">
         <v>392</v>
@@ -1023,15 +1025,15 @@
         <v>28</v>
       </c>
       <c r="D26" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="E26" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s">
         <v>27</v>
@@ -1040,49 +1042,49 @@
         <v>28</v>
       </c>
       <c r="D27" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="E27" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C28" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D28" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E28" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C29" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" t="s">
         <v>41</v>
       </c>
-      <c r="D29" t="s">
-        <v>38</v>
-      </c>
       <c r="E29" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B32" s="2"/>
     </row>

</xml_diff>